<commit_message>
[CCORDERO] changes performed to DenseNet architecture and analysys performed
</commit_message>
<xml_diff>
--- a/presicion_analisis_DenseNet.xlsx
+++ b/presicion_analisis_DenseNet.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BD9471-282A-4EDF-B6EA-4D658C8B4E69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA25032C-E68D-4C69-BAE1-8D4EA8039F88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6DenseNet0.00004" sheetId="1" r:id="rId1"/>
-    <sheet name="6DenseNet0.000009" sheetId="7" r:id="rId2"/>
-    <sheet name="6DenseNet0.00008" sheetId="8" r:id="rId3"/>
-    <sheet name="6DenseNet0.0001" sheetId="9" r:id="rId4"/>
-    <sheet name="6DenseNet0.0004" sheetId="10" r:id="rId5"/>
-    <sheet name="63DenseNet0.0001" sheetId="11" r:id="rId6"/>
+    <sheet name="6DenseNet0.00008" sheetId="8" r:id="rId2"/>
+    <sheet name="6DenseNet0.00012" sheetId="9" r:id="rId3"/>
+    <sheet name="6DenseNet0.00016" sheetId="10" r:id="rId4"/>
+    <sheet name="6DenseNet0.0002" sheetId="12" r:id="rId5"/>
+    <sheet name="63DenseNet0.00016" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,10 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -105,17 +104,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>751788</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>18165</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>237400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>53543</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19CF2CA7-B5B5-4718-A8EC-D0EA62DD63CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CADB03D-E430-4778-A2F0-D8D5381CDE7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -132,7 +131,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5495238" cy="7076190"/>
+          <a:ext cx="5800000" cy="7085714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -155,16 +154,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>418455</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>75308</xdr:rowOff>
+      <xdr:colOff>355866</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171934</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{047E2402-7870-45E5-98D4-0AF5C25CBA41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00F4008C-5C27-406D-B628-1FA0C543146F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -181,7 +180,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5161905" cy="7133333"/>
+          <a:ext cx="5123809" cy="7019048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -203,17 +202,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>224069</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>99992</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>760047</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>34496</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D53A0D13-2700-46C5-B955-BF8E106C9E7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12065D0B-CA73-4634-97A4-AAEF372BDE48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -230,7 +229,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5771429" cy="7780952"/>
+          <a:ext cx="4733333" cy="7066667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -252,17 +251,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>492739</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>42849</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>265971</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>101162</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD2FF614-5E60-495F-8F1B-700EEBFBD9B3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B3CB97E-AD3E-4670-97DA-F093640C7CE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -279,7 +278,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5247619" cy="7723809"/>
+          <a:ext cx="5828571" cy="7133333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -302,16 +301,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>692739</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>109516</xdr:rowOff>
+      <xdr:colOff>130834</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1013</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ABB284F-6D24-4285-B92F-FCC57C8780EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F433E33-B5A3-4439-BA6F-4A7C296622C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -328,7 +327,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5447619" cy="7790476"/>
+          <a:ext cx="4885714" cy="7133333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -351,16 +350,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>664168</xdr:colOff>
+      <xdr:colOff>549882</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>136274</xdr:rowOff>
+      <xdr:rowOff>117227</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B8E52AE-526C-4D00-8EAE-77B5BCF1B64A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95C745C3-1877-4C32-B65F-DE09B40DA714}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -377,7 +376,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5419048" cy="7085714"/>
+          <a:ext cx="5304762" cy="7066667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -689,7 +688,7 @@
   <dimension ref="J13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,31 +703,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63A6E58-9720-4BC3-820A-7586F29B7024}">
-  <dimension ref="I20"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I20" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED88CEAE-6060-47EC-A100-8959A438A288}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,12 +717,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE138D8-80C8-45F3-BC9A-0119FA3B16D4}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,12 +732,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C97DDA6-8A00-4536-8A24-7DD182C52558}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,12 +747,27 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FEB8AA-57A9-48FB-8716-CF5B76940D46}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF47F68-9F73-4104-8EBB-BA38A29B6E7B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N20" sqref="N19:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[CCORDERO] best hyperparameter analysis completed
</commit_message>
<xml_diff>
--- a/presicion_analisis_DenseNet.xlsx
+++ b/presicion_analisis_DenseNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA25032C-E68D-4C69-BAE1-8D4EA8039F88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F38A115-C34E-4264-B158-A53D1C052FC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6DenseNet0.00004" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="6DenseNet0.00016" sheetId="10" r:id="rId4"/>
     <sheet name="6DenseNet0.0002" sheetId="12" r:id="rId5"/>
     <sheet name="63DenseNet0.00016" sheetId="11" r:id="rId6"/>
+    <sheet name="6DenseNet0.00016_no_ReduceLR" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -377,6 +378,99 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="5304762" cy="7066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>725318</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>134918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FD8D5E2-C68C-47F9-BFC1-D30608B91C1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3895238" cy="2695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28076</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>18705</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE64AA3-A723-4D8B-9A80-67A7FF18FC5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4754880" y="0"/>
+          <a:ext cx="3990476" cy="2761905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -766,8 +860,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF47F68-9F73-4104-8EBB-BA38A29B6E7B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N20" sqref="N19:N20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3805CCF-A6D8-4C6D-9133-6D9371088ED2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[CCORDERO] DenseNet161 63 classes analysis added
</commit_message>
<xml_diff>
--- a/presicion_analisis_DenseNet.xlsx
+++ b/presicion_analisis_DenseNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F38A115-C34E-4264-B158-A53D1C052FC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F70BED-C287-4DA7-9E1E-4A3846C538EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6DenseNet0.00004" sheetId="1" r:id="rId1"/>
@@ -350,17 +350,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>549882</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>117227</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>640419</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171105</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95C745C3-1877-4C32-B65F-DE09B40DA714}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6CF012-2940-4326-A6AB-A99966EBC47C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -377,7 +377,51 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5304762" cy="7066667"/>
+          <a:ext cx="3819048" cy="2761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>640419</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133009</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B4BECD1-7302-4445-82B4-57428BF6F4C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3331029"/>
+          <a:ext cx="3819048" cy="2723809"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -861,7 +905,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,7 +920,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[CCORDERO] results with official dataset
</commit_message>
<xml_diff>
--- a/presicion_analisis_DenseNet.xlsx
+++ b/presicion_analisis_DenseNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F70BED-C287-4DA7-9E1E-4A3846C538EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349C542D-0110-4783-8A65-B3B7A123FF6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6DenseNet0.00004" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,17 +351,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>640419</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7666</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>171105</xdr:rowOff>
+      <xdr:rowOff>18724</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6CF012-2940-4326-A6AB-A99966EBC47C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A3C9B86-0BA9-4B49-985B-F7B73F00C3BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -377,7 +378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3819048" cy="2761905"/>
+          <a:ext cx="3980952" cy="2609524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -390,21 +391,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>640419</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>133009</xdr:rowOff>
+      <xdr:colOff>754704</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28248</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B4BECD1-7302-4445-82B4-57428BF6F4C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6731868-1CDE-4FF5-ACBD-66DB0F05A69C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -420,8 +421,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3331029"/>
-          <a:ext cx="3819048" cy="2723809"/>
+          <a:off x="0" y="3516086"/>
+          <a:ext cx="3933333" cy="2619048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -902,16 +903,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF47F68-9F73-4104-8EBB-BA38A29B6E7B}">
-  <dimension ref="A1"/>
+  <dimension ref="J17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J17" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -919,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3805CCF-A6D8-4C6D-9133-6D9371088ED2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[CCORDERO] last commit to DenseNet
</commit_message>
<xml_diff>
--- a/presicion_analisis_DenseNet.xlsx
+++ b/presicion_analisis_DenseNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349C542D-0110-4783-8A65-B3B7A123FF6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4899F716-8079-4BC0-A83D-2D18E5226F2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6DenseNet0.00004" sheetId="1" r:id="rId1"/>
@@ -351,17 +351,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>7666</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>18724</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217095</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>67607</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A3C9B86-0BA9-4B49-985B-F7B73F00C3BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D1038E3-6321-4D2D-B2A6-1A8703FB9F68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -378,7 +378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3980952" cy="2609524"/>
+          <a:ext cx="4952381" cy="3428571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -389,23 +389,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>754704</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>28248</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>711072</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>139738</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6731868-1CDE-4FF5-ACBD-66DB0F05A69C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6339A64C-287B-46BB-AC1D-6FD03CBFD202}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -421,8 +421,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3516086"/>
-          <a:ext cx="3933333" cy="2619048"/>
+          <a:off x="5524500" y="0"/>
+          <a:ext cx="4657143" cy="3323809"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -903,16 +903,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF47F68-9F73-4104-8EBB-BA38A29B6E7B}">
-  <dimension ref="J17"/>
+  <dimension ref="J17:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="10:11" x14ac:dyDescent="0.3">
       <c r="J17" s="2"/>
+    </row>
+    <row r="25" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[CCORDERO] categorical correction added
</commit_message>
<xml_diff>
--- a/presicion_analisis_DenseNet.xlsx
+++ b/presicion_analisis_DenseNet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4899F716-8079-4BC0-A83D-2D18E5226F2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57049503-A756-4230-BC51-A56D8112ABC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6DenseNet0.00004" sheetId="1" r:id="rId1"/>
@@ -906,7 +906,7 @@
   <dimension ref="J17:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[CCORDERO] Reorganizing and tensorboard examples added
</commit_message>
<xml_diff>
--- a/presicion_analisis_DenseNet.xlsx
+++ b/presicion_analisis_DenseNet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57049503-A756-4230-BC51-A56D8112ABC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB4FA59-BC09-4906-AB02-6C00479E2BAE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
@@ -351,17 +351,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>217095</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>67607</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>549167</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>126154</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D1038E3-6321-4D2D-B2A6-1A8703FB9F68}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79D1FB8B-3DB4-41BF-8EEA-D086A5BAC84A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -378,7 +378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="4952381" cy="3428571"/>
+          <a:ext cx="4495238" cy="3133333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -396,16 +396,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>711072</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>139738</xdr:rowOff>
+      <xdr:colOff>568215</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88059</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6339A64C-287B-46BB-AC1D-6FD03CBFD202}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86E5BFC4-B9F1-4E7A-BB1B-34BB89424907}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -422,7 +422,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524500" y="0"/>
-          <a:ext cx="4657143" cy="3323809"/>
+          <a:ext cx="4514286" cy="3095238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -906,7 +906,7 @@
   <dimension ref="J17:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>